<commit_message>
Cập nhật thêm thông tin vài mẫu thiết kế.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -180,6 +180,27 @@
   </si>
   <si>
     <t>Một đối tượng không thể tạo ngoài assembly --&gt; clone</t>
+  </si>
+  <si>
+    <t>Việc khởi tạo thực hiện duy nhất 1 lần</t>
+  </si>
+  <si>
+    <t>Chưa rõ</t>
+  </si>
+  <si>
+    <t>Quyết định quy trình chạy của các lớp theo thứ tự nhất định</t>
+  </si>
+  <si>
+    <t>Chuyên xử lý các hành động undo, redo</t>
+  </si>
+  <si>
+    <t>Quản lý định dạng date hoặc việc đọc dữ liệu từ bên ngoài của nhiều class</t>
+  </si>
+  <si>
+    <t>Quản lý kiểu danh sách nhiều phần tử</t>
+  </si>
+  <si>
+    <t>Điều phối thông điệp với các thể hiện khác nhau</t>
   </si>
 </sst>
 </file>
@@ -281,23 +302,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -606,106 +627,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -733,93 +754,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>49</v>
+      <c r="D5" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>49</v>
+      <c r="D6" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>49</v>
+      <c r="C7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -834,170 +857,180 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.875" customWidth="1"/>
+    <col min="3" max="3" width="62.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1026,108 +1059,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1154,62 +1187,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Nghiên cứu cơ bản xong phần design patterns.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -4,21 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="Creational" sheetId="2" r:id="rId2"/>
-    <sheet name="Behavioral" sheetId="3" r:id="rId3"/>
-    <sheet name="Structural" sheetId="4" r:id="rId4"/>
-    <sheet name="Suggest" sheetId="5" r:id="rId5"/>
+    <sheet name="DP" sheetId="2" r:id="rId2"/>
+    <sheet name="Suggest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -56,9 +54,6 @@
     <t>Có thể áp dụng</t>
   </si>
   <si>
-    <t>Khó áp dụng</t>
-  </si>
-  <si>
     <t>CÁC ĐỀ NGHỊ CẦN XEM XÉT</t>
   </si>
   <si>
@@ -167,9 +162,6 @@
     <t>Proxy Pattern</t>
   </si>
   <si>
-    <t>Đang nghiên cứu</t>
-  </si>
-  <si>
     <t>Tạo ra lớp cơ sở để quản lý các lớp</t>
   </si>
   <si>
@@ -201,13 +193,73 @@
   </si>
   <si>
     <t>Điều phối thông điệp với các thể hiện khác nhau</t>
+  </si>
+  <si>
+    <t>Khó áp dụng, có thể kết hợp với spring.NET</t>
+  </si>
+  <si>
+    <t>Thay đổi trạng thái (enum)bên trong 1 class mà không phá vỡ tính bao bọc của class đó</t>
+  </si>
+  <si>
+    <t>Thông báo thay đổi trạng thái ở đối tượng chính lên tất cả đối tượng con một cách tự động
+Thường dùng trong quan hệ một nhiều</t>
+  </si>
+  <si>
+    <t>Quản lý trạng thái sản phẩm tự động gọi hành vi A hoặc B theo điều kiện cho trước
+Ngăn dirty update hoặc update bất đồng bộ</t>
+  </si>
+  <si>
+    <t>Quản lý thuật toán khác nhau để dễ chỉnh sửa về sau</t>
+  </si>
+  <si>
+    <t>Đưa phần chung (thuộc tính, phương thức) lên bên trên thành lớp cơ sở</t>
+  </si>
+  <si>
+    <t>Bao bọc phần database transaction</t>
+  </si>
+  <si>
+    <t>Chuyển dữ liệu đầu vào theo định dạng cần thiết cho đầu ra
+Sử dụng phương thức của lớp khác mà không kế thừa trực tiếp</t>
+  </si>
+  <si>
+    <t>Cho phép một class dùng tính năng từ nhiều lớp khác mà không kế thừa trực tiếp</t>
+  </si>
+  <si>
+    <t>Các class có một phương thức cùng tên, cách xử lý khác nhau, không muốn gọi từng class thực hiện</t>
+  </si>
+  <si>
+    <t>Thêm một thành phần vào đối tượng mà không thao tác với đội tượng đó</t>
+  </si>
+  <si>
+    <t>Nhiều lớp có phương thức tạo thành một quy trình khi muốn gọi các phương thức đó theo thứ tự bên ngoài assembly --&gt; dùng interface</t>
+  </si>
+  <si>
+    <t>Hỗ trợ số lượng lớn các đối tượng nhỏ (như character) bằng cách chia sẻ giá trị chung</t>
+  </si>
+  <si>
+    <t>Có đối tượng ở domain khác nhưng không muốn khởi tạo nó trong domain cục bộ --&gt; dùng proxy kết nối 2 domain</t>
+  </si>
+  <si>
+    <t>Tham khảo từ: Design Patterns - Christopher G. Lasater</t>
+  </si>
+  <si>
+    <t>HiỆN TRẠNG</t>
+  </si>
+  <si>
+    <t>Đang xem xét</t>
+  </si>
+  <si>
+    <t>Thống nhất dùng VS2010</t>
+  </si>
+  <si>
+    <t>Vẫn để 3-tier 3-layer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +276,31 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -233,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -257,37 +334,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -297,26 +346,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -615,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -685,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -739,7 +794,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -748,56 +803,50 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -805,376 +854,343 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="42.75">
+      <c r="A16" s="2">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.5">
+      <c r="A17" s="2">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2">
+        <v>11</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15">
+      <c r="A21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" ht="28.5">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.375" customWidth="1"/>
-    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1183,66 +1199,81 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="41.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.25" customWidth="1"/>
+    <col min="3" max="3" width="67.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Cập nhật các kỹ thuật đã học.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Asynchronous (Web service)</t>
   </si>
   <si>
-    <t>Delegate &amp; Event</t>
-  </si>
-  <si>
     <t>Có thể áp dụng</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
   </si>
   <si>
     <t>Điều phối thông điệp với các thể hiện khác nhau</t>
-  </si>
-  <si>
-    <t>Khó áp dụng, có thể kết hợp với spring.NET</t>
   </si>
   <si>
     <t>Thay đổi trạng thái (enum)bên trong 1 class mà không phá vỡ tính bao bọc của class đó</t>
@@ -253,6 +247,39 @@
   </si>
   <si>
     <t>Vẫn để 3-tier 3-layer</t>
+  </si>
+  <si>
+    <t>Delegate &amp; Event (Public &amp; Subscriber)</t>
+  </si>
+  <si>
+    <t>Message Transformation</t>
+  </si>
+  <si>
+    <t>5 mẫu thiết kế</t>
+  </si>
+  <si>
+    <t>11 mẫu thiết kế</t>
+  </si>
+  <si>
+    <t>7 mẫu thiết kế</t>
+  </si>
+  <si>
+    <t>Mô hình Model-Controller-View</t>
+  </si>
+  <si>
+    <t>Khó áp dụng, có thể dùng với PureMVC hoặc MVC#</t>
+  </si>
+  <si>
+    <t>Tạo đối tượng bên client khi dùng web serivce</t>
+  </si>
+  <si>
+    <t>Bất đồng bộ khi gọi các phương thức của web service</t>
+  </si>
+  <si>
+    <t>Phần xử lý sự kiện nằm riêng trong một class</t>
+  </si>
+  <si>
+    <t>Đọc file XML và chuyển thành giao diện</t>
   </si>
 </sst>
 </file>
@@ -346,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,17 +389,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,38 +698,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.375" customWidth="1"/>
-    <col min="3" max="3" width="51.5" customWidth="1"/>
+    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" ht="15">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -707,10 +742,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>78</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -718,10 +756,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>79</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -729,10 +770,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>80</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -740,10 +784,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -751,10 +798,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>83</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -762,30 +812,59 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>84</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>85</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -809,47 +888,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="15">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="A3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -857,13 +936,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -871,13 +950,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -885,13 +964,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -899,35 +978,35 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -935,13 +1014,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -949,13 +1028,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -963,13 +1042,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -977,13 +1056,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -991,27 +1070,27 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="42.75">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.5">
       <c r="A16" s="2">
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5">
@@ -1019,13 +1098,13 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1033,13 +1112,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1047,13 +1126,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1061,35 +1140,35 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15">
+      <c r="A21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="A21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="28.5">
       <c r="A22" s="2">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1097,13 +1176,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1111,13 +1190,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1125,13 +1204,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1139,13 +1218,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1153,13 +1232,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1167,13 +1246,13 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1204,11 +1283,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="15">
@@ -1219,10 +1298,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>74</v>
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1230,13 +1309,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1244,13 +1323,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1258,13 +1337,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
Cập nhật báo cáo. Cài đặt mẫu singleton.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Một đối tượng không thể tạo ngoài assembly --&gt; clone</t>
-  </si>
-  <si>
-    <t>Việc khởi tạo thực hiện duy nhất 1 lần</t>
   </si>
   <si>
     <t>Chưa rõ</t>
@@ -280,6 +277,30 @@
   </si>
   <si>
     <t>Đọc file XML và chuyển thành giao diện</t>
+  </si>
+  <si>
+    <t>3-layer</t>
+  </si>
+  <si>
+    <t>3-tier</t>
+  </si>
+  <si>
+    <t>3-layer: DAO, BUS, Presentation</t>
+  </si>
+  <si>
+    <t>Đã áp dụng</t>
+  </si>
+  <si>
+    <t>3-tier: DAL_WS, BUS_WS, QLBSX</t>
+  </si>
+  <si>
+    <t>Việc khởi tạo thực hiện duy nhất 1 lần trong lúc kết nối CSDL (QLBSX_DAL_WS --&gt; DataProvider.cs)</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>Hướng đối tượng, có lớp đối tượng xử lý riêng các phương thức liên quan</t>
   </si>
 </sst>
 </file>
@@ -408,7 +429,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -698,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -742,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -756,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -770,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -784,10 +842,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -798,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -812,7 +870,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -823,10 +881,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -837,10 +895,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -850,17 +908,43 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -876,7 +960,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -889,7 +973,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -956,7 +1040,7 @@
         <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -970,7 +1054,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -981,10 +1065,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15">
@@ -1003,10 +1087,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1017,10 +1101,10 @@
         <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1031,10 +1115,10 @@
         <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1045,10 +1129,10 @@
         <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1059,10 +1143,10 @@
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1073,10 +1157,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.5">
@@ -1087,10 +1171,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5">
@@ -1101,10 +1185,10 @@
         <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1115,10 +1199,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1129,7 +1213,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>10</v>
@@ -1143,10 +1227,10 @@
         <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15">
@@ -1165,7 +1249,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>10</v>
@@ -1179,10 +1263,10 @@
         <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1193,10 +1277,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1207,7 +1291,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>10</v>
@@ -1221,10 +1305,10 @@
         <v>44</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1235,10 +1319,10 @@
         <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1249,7 +1333,7 @@
         <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>10</v>
@@ -1262,6 +1346,17 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Đã áp dụng">
+      <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Có thể áp dụng">
+      <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Chưa rõ">
+      <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1301,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1315,7 +1410,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1329,7 +1424,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1343,7 +1438,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
Chỉnh sửa code theo đúng mẫu singleton. Chỉnh sửa CSDL phần năm của ngày hết hạn. Bổ sung Technique.xlsx.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>Hướng đối tượng, có lớp đối tượng xử lý riêng các phương thức liên quan</t>
+  </si>
+  <si>
+    <t>Giao diện động</t>
+  </si>
+  <si>
+    <t>Phần thêm/cập nhật/tra cứu biển số 3 loại xe</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -463,6 +481,30 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -756,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -934,7 +976,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>92</v>
@@ -945,11 +987,57 @@
       <c r="D13" s="2" t="s">
         <v>89</v>
       </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>$D$9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$D$13</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1347,13 +1435,13 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Chỉnh sửa DAL, BUS và Presentation áp dụng Deaign Patterns. Chỉnh sửa Technique.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -159,16 +159,10 @@
     <t>Proxy Pattern</t>
   </si>
   <si>
-    <t>Tạo ra lớp cơ sở để quản lý các lớp</t>
-  </si>
-  <si>
     <t>nhiều lớp cần interface chung đến một phương thức factory để tạo thuộc tính bên trong</t>
   </si>
   <si>
     <t>Một lớp cần khởi tạo nhiều thuộc tính và theo thứ tự</t>
-  </si>
-  <si>
-    <t>Một đối tượng không thể tạo ngoài assembly --&gt; clone</t>
   </si>
   <si>
     <t>Chưa rõ</t>
@@ -200,19 +194,9 @@
 Ngăn dirty update hoặc update bất đồng bộ</t>
   </si>
   <si>
-    <t>Quản lý thuật toán khác nhau để dễ chỉnh sửa về sau</t>
-  </si>
-  <si>
-    <t>Đưa phần chung (thuộc tính, phương thức) lên bên trên thành lớp cơ sở</t>
-  </si>
-  <si>
     <t>Bao bọc phần database transaction</t>
   </si>
   <si>
-    <t>Chuyển dữ liệu đầu vào theo định dạng cần thiết cho đầu ra
-Sử dụng phương thức của lớp khác mà không kế thừa trực tiếp</t>
-  </si>
-  <si>
     <t>Cho phép một class dùng tính năng từ nhiều lớp khác mà không kế thừa trực tiếp</t>
   </si>
   <si>
@@ -294,9 +278,6 @@
     <t>3-tier: DAL_WS, BUS_WS, QLBSX</t>
   </si>
   <si>
-    <t>Việc khởi tạo thực hiện duy nhất 1 lần trong lúc kết nối CSDL (QLBSX_DAL_WS --&gt; DataProvider.cs)</t>
-  </si>
-  <si>
     <t>OOP</t>
   </si>
   <si>
@@ -307,13 +288,173 @@
   </si>
   <si>
     <t>Phần thêm/cập nhật/tra cứu biển số 3 loại xe</t>
+  </si>
+  <si>
+    <t>Cloud Computing</t>
+  </si>
+  <si>
+    <t>Dành riêng cho ứng dụng web</t>
+  </si>
+  <si>
+    <t>Không thể áp dụng</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quản lý việc khởi tạo một đối tượng duy nhất một lần, sử dụng static, chỉ cho get, không cho set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Việc khởi tạo thực hiện duy nhất 1 lần trong lúc kết nối CSDL (QLBSX_DAL_WS --&gt; DataProvider.cs)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tạo ra lớp Factory để quản lý các lớp, có lớp cơ sở là Abstract Class.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+BienSoXe là abstract class, BienSoXeFactory quản lý việc thêm, xóa, sửa BienSoXe.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Một đối tượng không thể tạo ngoài assembly --&gt; clone. Sao chép bản mẫu đối tượng.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trong lớp BienSoXe có phương thức trừu tượng Clone, các lớp dẫn xuất cài đặt lại phương thức này.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quản lý thuật toán khác nhau để dễ chỉnh sửa về sau.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trong BienSoXe có abstract method GetInfo, các lớp kế thừa từ lớp này (BienSoXeMoto) sẽ cài đặt lại phương thức này.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đưa một template method (khung) bên trong có một số phương thức mà lớp con sẽ cài đặt riêng.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+BienXoSe là abstract class có phương thức "Add" là template method, bên trong phương thức này gọi đến phương thức GetInfo.
+Cách thực hiện của phương thức GetInfo sẽ tùy vào các lớp dẫn xuất.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chuyển dữ liệu đầu vào theo định dạng cần thiết cho đầu ra.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trong class BienSoXeMoto có phương thức ConvertToMoto, có mục địch là để điểm kiểm tra đầu vào (object) có phải là BienSoXeMoto hay không, nếu có thì trả về BienSoXeMoto, ngược lại trả về null</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +491,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -400,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,11 +580,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -464,6 +628,18 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -476,6 +652,18 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -505,6 +693,210 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -801,7 +1193,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -842,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -856,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -870,7 +1262,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -884,10 +1276,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -898,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -912,7 +1304,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -923,10 +1315,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -937,10 +1329,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -951,13 +1343,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -965,13 +1357,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -979,13 +1371,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -993,22 +1385,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
@@ -1031,10 +1429,10 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>$D$13</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1048,7 +1446,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1061,7 +1459,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1089,18 +1487,18 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="29.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
+      <c r="C4" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1111,7 +1509,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -1125,38 +1523,38 @@
         <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:4" ht="29.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
+      <c r="C7" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>91</v>
+      <c r="C8" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15">
@@ -1175,10 +1573,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1189,10 +1587,10 @@
         <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1203,10 +1601,10 @@
         <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1217,10 +1615,10 @@
         <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1231,10 +1629,10 @@
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1245,10 +1643,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.5">
@@ -1259,10 +1657,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5">
@@ -1273,38 +1671,38 @@
         <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.25">
       <c r="A18" s="2">
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>60</v>
+      <c r="C18" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.5">
       <c r="A19" s="2">
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>61</v>
+      <c r="C19" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1315,10 +1713,10 @@
         <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15">
@@ -1329,18 +1727,18 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" ht="28.5">
+    <row r="22" spans="1:4" ht="43.5">
       <c r="A22" s="2">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>63</v>
+      <c r="C22" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1351,10 +1749,10 @@
         <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1365,10 +1763,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1379,7 +1777,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>10</v>
@@ -1393,10 +1791,10 @@
         <v>44</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1407,10 +1805,10 @@
         <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1421,7 +1819,7 @@
         <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>10</v>
@@ -1435,13 +1833,13 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1455,7 +1853,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1484,7 +1882,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1498,7 +1896,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1512,7 +1910,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1526,7 +1924,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
1.	Update ArchitectureReport.doc: viết báo cáo tất cả các phần 2.	Viết code cho Distributed Objects: thêm class DOMain, bên trong F_AMain_QLBSX chỉ gọi thông qua đối tượng này. 3.	Update Technique.xlsx 4.	Các hình vẽ đều để trong: ClassDiagram.vsd
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -251,9 +251,6 @@
     <t>Khó áp dụng, có thể dùng với PureMVC hoặc MVC#</t>
   </si>
   <si>
-    <t>Tạo đối tượng bên client khi dùng web serivce</t>
-  </si>
-  <si>
     <t>Bất đồng bộ khi gọi các phương thức của web service</t>
   </si>
   <si>
@@ -304,7 +301,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -315,7 +312,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -329,7 +326,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -340,7 +337,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -354,7 +351,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -365,7 +362,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -379,7 +376,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -390,7 +387,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -404,7 +401,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -415,7 +412,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -430,7 +427,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -441,7 +438,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -449,16 +446,34 @@
 Trong class BienSoXeMoto có phương thức ConvertToMoto, có mục địch là để điểm kiểm tra đầu vào (object) có phải là BienSoXeMoto hay không, nếu có thì trả về BienSoXeMoto, ngược lại trả về null</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tạo đối tượng bên client khi dùng web serivce
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tạo ra lớp DOMain để thao tác với webservice khi đó
+F_Amain_QLBSX chỉ việc gọi thông qua</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -466,7 +481,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -474,7 +489,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -482,7 +497,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -491,7 +506,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -499,9 +514,17 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -571,6 +594,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,266 +606,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1193,26 +964,26 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1282,18 +1053,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="60">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>77</v>
+      <c r="C7" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1304,7 +1075,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1318,7 +1089,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -1332,7 +1103,7 @@
         <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -1343,13 +1114,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1357,13 +1128,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1371,13 +1142,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1385,13 +1156,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1399,13 +1170,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1429,10 +1200,10 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$D$13</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1449,23 +1220,23 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1479,26 +1250,26 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" ht="29.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>94</v>
+      <c r="C4" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1529,41 +1300,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29.25">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>95</v>
+      <c r="C7" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>93</v>
+      <c r="C8" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
@@ -1649,7 +1420,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.5">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="2">
         <v>7</v>
       </c>
@@ -1663,7 +1434,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.5">
+    <row r="17" spans="1:4" ht="30">
       <c r="A17" s="2">
         <v>8</v>
       </c>
@@ -1677,32 +1448,32 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.25">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" s="2">
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>96</v>
+      <c r="C18" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="43.5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60">
       <c r="A19" s="2">
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>97</v>
+      <c r="C19" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1719,26 +1490,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" ht="43.5">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" ht="45">
       <c r="A22" s="2">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>98</v>
+      <c r="C22" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1833,13 +1604,13 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1856,22 +1627,22 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
1.	Update ArchitectureReport.doc: Message Transformation 2.	Viết code cho Message Transformation, thêm file configButton.xml 3.	Update Technique.xlsx 4.	Update ClassDiagram.vsd
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>Phần xử lý sự kiện nằm riêng trong một class</t>
-  </si>
-  <si>
-    <t>Đọc file XML và chuyển thành giao diện</t>
   </si>
   <si>
     <t>3-layer</t>
@@ -462,6 +459,25 @@
       </rPr>
       <t>Tạo ra lớp DOMain để thao tác với webservice khi đó
 F_Amain_QLBSX chỉ việc gọi thông qua</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Đọc file XML và chuyển thành giao diện:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chỉ demo ở main form: cấu hình các button ra file xml
+configButton.xml, đọc file xml lên và phát sinh ra button
+và cả sự kiện của button đó.</t>
     </r>
   </si>
 </sst>
@@ -610,7 +626,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -964,7 +1004,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1061,10 +1101,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1095,18 +1135,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="90">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>79</v>
+      <c r="C10" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1114,13 +1154,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1128,13 +1168,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1142,13 +1182,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1156,13 +1196,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1170,13 +1210,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1200,10 +1240,10 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$D$13</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1266,10 +1306,10 @@
         <v>22</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1308,10 +1348,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30">
@@ -1322,10 +1362,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1456,10 +1496,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="60">
@@ -1470,10 +1510,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1506,10 +1546,10 @@
         <v>40</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1604,13 +1644,13 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Cập nhật mã nguồn, chỉnh sửa lớp trên Presentation. Chỉnh sửa báo cáo, các hình ảnh trong Design Patterns. Cập nhật các tài liệu tham khảo.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -298,7 +298,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -309,7 +309,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -323,7 +323,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -334,7 +334,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -348,7 +348,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -359,7 +359,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -373,7 +373,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -384,7 +384,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -398,7 +398,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -409,7 +409,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -424,7 +424,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -435,7 +435,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -453,13 +453,25 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Tạo ra lớp DOMain để thao tác với webservice khi đó
 F_Amain_QLBSX chỉ việc gọi thông qua</t>
     </r>
+  </si>
+  <si>
+    <t>RESTful Web service</t>
+  </si>
+  <si>
+    <t>Sử dụng REST thay SOAP</t>
+  </si>
+  <si>
+    <t>Plug-in</t>
+  </si>
+  <si>
+    <t>Code Generator</t>
   </si>
   <si>
     <r>
@@ -471,13 +483,11 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Chỉ demo ở main form: cấu hình các button ra file xml
-configButton.xml, đọc file xml lên và phát sinh ra button
-và cả sự kiện của button đó.</t>
+      <t>Chỉ demo ở main form: cấu hình các button ra file configButton.xml, đọc file xml lên và phát sinh ra button và cả sự kiện của button đó.</t>
     </r>
   </si>
 </sst>
@@ -489,7 +499,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -497,7 +507,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -505,7 +515,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -513,7 +523,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -522,7 +532,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -530,7 +540,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -539,7 +549,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -588,16 +598,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,7 +618,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -622,35 +638,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1001,249 +996,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.125" customWidth="1"/>
+    <col min="4" max="4" width="43.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="44.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="2" t="s">
+    <row r="10" spans="1:4" ht="44.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="2" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="2" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2">
+    <row r="18" spans="1:4">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$D$13</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1260,379 +1277,379 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="2">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" ht="29.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="2">
+    <row r="7" spans="1:4" ht="29.25">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" s="2">
+    <row r="8" spans="1:4" ht="29.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>6</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="A16" s="2">
+    <row r="16" spans="1:4" ht="28.5">
+      <c r="A16" s="1">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="2">
+    <row r="17" spans="1:4" ht="28.5">
+      <c r="A17" s="1">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30">
-      <c r="A18" s="2">
+    <row r="18" spans="1:4" ht="29.25">
+      <c r="A18" s="1">
         <v>9</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60">
-      <c r="A19" s="2">
+    <row r="19" spans="1:4" ht="43.5">
+      <c r="A19" s="1">
         <v>10</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>11</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:4" ht="15">
+      <c r="A21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="A22" s="2">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" ht="43.5">
+      <c r="A22" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>2</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>3</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>4</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>5</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>6</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>7</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1644,13 +1661,13 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1667,84 +1684,84 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Áp dụng Delegate & Event. Áp dụng Asynchronous web service. Viết báo cáo cho 2 phần trên.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -645,7 +645,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -999,7 +1023,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1113,7 +1137,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1127,7 +1151,7 @@
         <v>78</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="44.25">
@@ -1257,10 +1281,10 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$D$13</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1661,13 +1685,13 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Bổ sung Memento Pattern.
</commit_message>
<xml_diff>
--- a/Technique.xlsx
+++ b/Technique.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>CÁC KỸ THUẬT ĐÃ HỌC</t>
   </si>
@@ -489,6 +489,9 @@
       </rPr>
       <t>Chỉ demo ở main form: cấu hình các button ra file configButton.xml, đọc file xml lên và phát sinh ra button và cả sự kiện của button đó.</t>
     </r>
+  </si>
+  <si>
+    <t>Khó áp dụng</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -674,6 +689,54 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -684,6 +747,28 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
@@ -710,6 +795,30 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -722,11 +831,359 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1023,7 +1480,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1281,11 +1738,14 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$D$13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Có thể áp dụng"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1364,7 +1824,7 @@
         <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1378,7 +1838,7 @@
         <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29.25">
@@ -1428,7 +1888,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1442,7 +1902,7 @@
         <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1456,7 +1916,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1470,7 +1930,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1484,7 +1944,7 @@
         <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1498,7 +1958,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.5">
@@ -1604,7 +2064,7 @@
         <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1618,7 +2078,7 @@
         <v>60</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1646,7 +2106,7 @@
         <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1660,7 +2120,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1685,14 +2145,17 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Đã áp dụng">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Đã áp dụng">
       <formula>NOT(ISERROR(SEARCH("Đã áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Có thể áp dụng">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Có thể áp dụng">
       <formula>NOT(ISERROR(SEARCH("Có thể áp dụng",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Chưa rõ">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Chưa rõ">
       <formula>NOT(ISERROR(SEARCH("Chưa rõ",D1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"Khó áp dụng"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>